<commit_message>
Added UsesHeaderNumber  - Added header number tests  - Upgraded LightweightExcelReader version
</commit_message>
<xml_diff>
--- a/ExcelToEnumerable.Tests/TestSpreadsheets/TestSpreadsheet1.xlsx
+++ b/ExcelToEnumerable.Tests/TestSpreadsheets/TestSpreadsheet1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="CustomColumnName" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="BadHeaderNames" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="EmptyColumnNames" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="No Header Works" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
   <si>
     <t xml:space="preserve">String</t>
   </si>
@@ -103,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">Decimalzz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value2</t>
   </si>
 </sst>
 </file>
@@ -214,7 +221,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -268,6 +275,46 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>3456</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -286,7 +333,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -358,7 +405,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.6"/>
@@ -446,7 +493,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -526,7 +573,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -597,11 +644,11 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -693,7 +740,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -773,7 +820,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -845,7 +892,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>